<commit_message>
Remove levitation ski forces and fix some variable names
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/Trajectory Sims/18-19 Trajectory Sim/Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D979BB9-5D6E-6B46-88FE-202702663E0E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9500F08-996E-7C4F-AE5A-90D9EFE0833B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31989,7 +31989,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -32187,7 +32187,7 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Adding the 'Maximum' for title Angular Acceleration
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="6" r:id="rId1"/>
@@ -259,9 +259,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Angular Acceleration </t>
-  </si>
-  <si>
     <t>𝛼</t>
   </si>
   <si>
@@ -290,6 +287,9 @@
   </si>
   <si>
     <t>Pod Parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum Angular Acceleration </t>
   </si>
 </sst>
 </file>
@@ -847,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1100,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1179,36 +1179,36 @@
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="C5" s="25" t="s">
         <v>55</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>56</v>
       </c>
       <c r="D5" s="25">
         <v>111.755</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="C6" s="25" t="s">
         <v>59</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>60</v>
       </c>
       <c r="D6" s="25">
         <v>10000</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1235,7 +1235,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -1266,7 +1266,7 @@
     </row>
     <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>9</v>
@@ -1326,7 +1326,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>

</xml_diff>

<commit_message>
Edit the Matlab variables
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -262,9 +262,6 @@
     <t>𝛼</t>
   </si>
   <si>
-    <t>alpha</t>
-  </si>
-  <si>
     <t>rad/sˆ2</t>
   </si>
   <si>
@@ -274,9 +271,6 @@
     <t>f</t>
   </si>
   <si>
-    <t>rpm</t>
-  </si>
-  <si>
     <t>RPM</t>
   </si>
   <si>
@@ -290,6 +284,12 @@
   </si>
   <si>
     <t xml:space="preserve">Maximum Angular Acceleration </t>
+  </si>
+  <si>
+    <t>m_alpha</t>
+  </si>
+  <si>
+    <t>m_rpm</t>
   </si>
 </sst>
 </file>
@@ -1179,36 +1179,36 @@
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>54</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D5" s="25">
         <v>111.755</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="25" t="s">
-        <v>58</v>
-      </c>
       <c r="C6" s="25" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D6" s="25">
         <v>10000</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1235,7 +1235,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -1266,7 +1266,7 @@
     </row>
     <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>9</v>
@@ -1326,7 +1326,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>

</xml_diff>

<commit_message>
Removed Halbach array parameters and cleaned up namespace
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SimonaProkopovic/Documents/MATLAB/Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5035813-8355-2E43-B324-1D4E831C2948}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" activeTab="1"/>
+    <workbookView xWindow="1040" yWindow="-19400" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="6" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Tube" sheetId="8" r:id="rId3"/>
     <sheet name="Pod" sheetId="9" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>Parameters</t>
   </si>
@@ -265,9 +266,6 @@
     <t>rad/sˆ2</t>
   </si>
   <si>
-    <t>Maximum Rotational Frequency</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
@@ -283,20 +281,35 @@
     <t>Pod Parameters</t>
   </si>
   <si>
-    <t xml:space="preserve">Maximum Angular Acceleration </t>
-  </si>
-  <si>
     <t>m_alpha</t>
   </si>
   <si>
     <t>m_rpm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max. Angular Acceleration </t>
+  </si>
+  <si>
+    <t>Max. Rotational Frequency</t>
+  </si>
+  <si>
+    <t>Max. Angular Velocity</t>
+  </si>
+  <si>
+    <t>⍵</t>
+  </si>
+  <si>
+    <t>m_omega</t>
+  </si>
+  <si>
+    <t>rad/s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -436,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -501,7 +514,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -521,6 +533,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -533,7 +551,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -844,34 +862,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="34" style="1" customWidth="1"/>
     <col min="2" max="6" width="18.6640625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:9" ht="20">
+      <c r="A1" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-    </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+    </row>
+    <row r="2" spans="1:9" ht="18">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -894,7 +912,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="18">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -914,7 +932,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="20">
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
@@ -935,7 +953,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="18">
       <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
@@ -956,7 +974,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="20">
       <c r="A6" s="8" t="s">
         <v>22</v>
       </c>
@@ -977,7 +995,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="18">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
@@ -998,7 +1016,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="20">
       <c r="A8" s="8" t="s">
         <v>28</v>
       </c>
@@ -1016,7 +1034,7 @@
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -1025,7 +1043,7 @@
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -1034,7 +1052,7 @@
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -1043,7 +1061,7 @@
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="B14" s="13"/>
       <c r="C14" s="16"/>
       <c r="D14" s="13"/>
@@ -1052,7 +1070,7 @@
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -1061,7 +1079,7 @@
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -1070,7 +1088,7 @@
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8">
       <c r="B17" s="17"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -1079,7 +1097,7 @@
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8">
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -1097,31 +1115,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="39" style="1" customWidth="1"/>
     <col min="2" max="6" width="19.33203125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:6" ht="21" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+    </row>
+    <row r="2" spans="1:6" ht="18">
       <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1159,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="20">
       <c r="A3" s="22" t="s">
         <v>6</v>
       </c>
@@ -1159,7 +1177,7 @@
       </c>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="18">
       <c r="A4" s="22" t="s">
         <v>14</v>
       </c>
@@ -1176,40 +1194,6 @@
         <v>16</v>
       </c>
       <c r="F4" s="23"/>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="25">
-        <v>111.755</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="25">
-        <v>10000</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>58</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1220,53 +1204,53 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="7" width="20.83203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:7" ht="21">
+      <c r="A1" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:7" ht="19">
+      <c r="A2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="27"/>
+    </row>
+    <row r="3" spans="1:7" ht="19">
+      <c r="A3" s="23" t="s">
         <v>59</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="28"/>
-    </row>
-    <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>60</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>9</v>
@@ -1274,7 +1258,7 @@
       <c r="C3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="28">
         <v>1264.92</v>
       </c>
       <c r="E3" s="23" t="s">
@@ -1283,23 +1267,23 @@
       <c r="F3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="28"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="G3" s="27"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1310,165 +1294,223 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="20" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.83203125" style="1" customWidth="1"/>
     <col min="2" max="6" width="14.1640625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:6" ht="21" customHeight="1">
+      <c r="A1" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" ht="18">
+      <c r="A2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18">
+      <c r="A3" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="30">
+        <v>450</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" ht="18">
+      <c r="A4" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="30">
+        <v>0.09</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" ht="18">
+      <c r="A5" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="30">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" ht="18">
+      <c r="A6" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="30">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" ht="18">
+      <c r="A7" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="30">
+        <v>5</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" ht="18">
+      <c r="A8" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="30">
+        <v>0.05</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" ht="18">
+      <c r="A9" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="24">
+        <v>10000</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:6" ht="18">
+      <c r="A10" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="31">
+        <f>D9*2*PI()/60</f>
+        <v>1047.1975511965977</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18">
+      <c r="A11" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="31">
-        <v>450</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="23"/>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="31">
-        <v>0.09</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="23"/>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="31">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="23"/>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="31">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="E6" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="23"/>
-    </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="31">
-        <v>5</v>
-      </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="23"/>
-    </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="31">
-        <v>0.05</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="23"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D11" s="24">
+        <v>111.755</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="32"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="32"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="32"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="32"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="32"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
@@ -1477,7 +1519,7 @@
       <c r="G17" s="15"/>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -1486,7 +1528,7 @@
       <c r="G18" s="15"/>
       <c r="H18" s="17"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -1495,7 +1537,7 @@
       <c r="G19" s="15"/>
       <c r="H19" s="17"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -1504,7 +1546,7 @@
       <c r="G20" s="15"/>
       <c r="H20" s="17"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -1513,7 +1555,7 @@
       <c r="G21" s="15"/>
       <c r="H21" s="17"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -1522,7 +1564,7 @@
       <c r="G22" s="15"/>
       <c r="H22" s="17"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -1531,7 +1573,7 @@
       <c r="G23" s="15"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
@@ -1540,7 +1582,7 @@
       <c r="G24" s="15"/>
       <c r="H24" s="17"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>

</xml_diff>

<commit_message>
Updated torque and power calculations
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5035813-8355-2E43-B324-1D4E831C2948}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90417634-7DED-0E42-8628-6C13CDEF2620}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="-19400" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="440" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Tube" sheetId="8" r:id="rId3"/>
     <sheet name="Pod" sheetId="9" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -865,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -964,7 +964,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="9">
-        <v>0.01</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>12</v>
@@ -1297,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1349,7 +1349,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="30">
-        <v>450</v>
+        <v>300</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>32</v>
@@ -1367,7 +1367,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="30">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>12</v>
@@ -1385,7 +1385,7 @@
         <v>36</v>
       </c>
       <c r="D5" s="30">
-        <v>0.14799999999999999</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="E5" s="30" t="s">
         <v>12</v>
@@ -1403,7 +1403,7 @@
         <v>38</v>
       </c>
       <c r="D6" s="30">
-        <v>6.0000000000000001E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="E6" s="30" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Updated power calculations and added plots
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90417634-7DED-0E42-8628-6C13CDEF2620}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E93AD0F-4D11-6844-9F08-B33BD49A3E14}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="440" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="460" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="6" r:id="rId1"/>
@@ -865,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1297,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Added documentation and fixed EmBrakes
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artis\Documents\GitHub\dynamics-2018\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Music/temp/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4CEABC-C137-495A-BF87-016FE9802C93}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8869E6D-5E8F-2A49-99D5-9DAB4507EACD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1458" windowWidth="28800" windowHeight="16158" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1460" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -871,18 +870,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="34" style="1" customWidth="1"/>
     <col min="2" max="6" width="18.6640625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.100000000000001">
+    <row r="1" spans="1:9" ht="20">
       <c r="A1" s="33" t="s">
         <v>43</v>
       </c>
@@ -895,7 +894,7 @@
       <c r="H1" s="33"/>
       <c r="I1" s="33"/>
     </row>
-    <row r="2" spans="1:9" ht="17.7">
+    <row r="2" spans="1:9" ht="18">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -918,7 +917,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="17.399999999999999">
+    <row r="3" spans="1:9" ht="18">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -938,7 +937,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="21">
+    <row r="4" spans="1:9" ht="20">
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
@@ -959,7 +958,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.7">
+    <row r="5" spans="1:9" ht="18">
       <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
@@ -980,7 +979,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="19.8">
+    <row r="6" spans="1:9" ht="20">
       <c r="A6" s="8" t="s">
         <v>22</v>
       </c>
@@ -1001,7 +1000,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="17.7">
+    <row r="7" spans="1:9" ht="18">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
@@ -1022,7 +1021,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="21">
+    <row r="8" spans="1:9" ht="20">
       <c r="A8" s="8" t="s">
         <v>28</v>
       </c>
@@ -1128,7 +1127,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="39" style="1" customWidth="1"/>
     <col min="2" max="6" width="19.33203125" style="1" customWidth="1"/>
@@ -1145,7 +1144,7 @@
       <c r="E1" s="34"/>
       <c r="F1" s="34"/>
     </row>
-    <row r="2" spans="1:6" ht="17.7">
+    <row r="2" spans="1:6" ht="18">
       <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
@@ -1165,7 +1164,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19.8">
+    <row r="3" spans="1:6" ht="20">
       <c r="A3" s="22" t="s">
         <v>6</v>
       </c>
@@ -1183,7 +1182,7 @@
       </c>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:6" ht="17.399999999999999">
+    <row r="4" spans="1:6" ht="18">
       <c r="A4" s="22" t="s">
         <v>14</v>
       </c>
@@ -1217,13 +1216,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="7" width="20.83203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.399999999999999">
+    <row r="1" spans="1:7" ht="21">
       <c r="A1" s="34" t="s">
         <v>58</v>
       </c>
@@ -1233,7 +1232,7 @@
       <c r="E1" s="35"/>
       <c r="F1" s="15"/>
     </row>
-    <row r="2" spans="1:7" ht="18.3">
+    <row r="2" spans="1:7" ht="19">
       <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
@@ -1254,7 +1253,7 @@
       </c>
       <c r="G2" s="27"/>
     </row>
-    <row r="3" spans="1:7" ht="18.3">
+    <row r="3" spans="1:7" ht="19">
       <c r="A3" s="23" t="s">
         <v>59</v>
       </c>
@@ -1303,11 +1302,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="37.83203125" style="1" customWidth="1"/>
     <col min="2" max="6" width="14.1640625" style="1" customWidth="1"/>
@@ -1324,7 +1323,7 @@
       <c r="E1" s="35"/>
       <c r="F1" s="15"/>
     </row>
-    <row r="2" spans="1:6" ht="17.399999999999999">
+    <row r="2" spans="1:6" ht="18">
       <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
@@ -1344,7 +1343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.399999999999999">
+    <row r="3" spans="1:6" ht="18">
       <c r="A3" s="30" t="s">
         <v>30</v>
       </c>
@@ -1362,7 +1361,7 @@
       </c>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:6" ht="17.399999999999999">
+    <row r="4" spans="1:6" ht="18">
       <c r="A4" s="30" t="s">
         <v>33</v>
       </c>
@@ -1380,7 +1379,7 @@
       </c>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6" ht="17.399999999999999">
+    <row r="5" spans="1:6" ht="18">
       <c r="A5" s="30" t="s">
         <v>35</v>
       </c>
@@ -1398,7 +1397,7 @@
       </c>
       <c r="F5" s="23"/>
     </row>
-    <row r="6" spans="1:6" ht="17.399999999999999">
+    <row r="6" spans="1:6" ht="18">
       <c r="A6" s="30" t="s">
         <v>37</v>
       </c>
@@ -1416,7 +1415,7 @@
       </c>
       <c r="F6" s="23"/>
     </row>
-    <row r="7" spans="1:6" ht="17.399999999999999">
+    <row r="7" spans="1:6" ht="18">
       <c r="A7" s="30" t="s">
         <v>39</v>
       </c>
@@ -1432,7 +1431,7 @@
       <c r="E7" s="30"/>
       <c r="F7" s="23"/>
     </row>
-    <row r="8" spans="1:6" ht="17.399999999999999">
+    <row r="8" spans="1:6" ht="18">
       <c r="A8" s="30" t="s">
         <v>41</v>
       </c>
@@ -1450,7 +1449,7 @@
       </c>
       <c r="F8" s="23"/>
     </row>
-    <row r="9" spans="1:6" ht="17.7">
+    <row r="9" spans="1:6" ht="18">
       <c r="A9" s="31" t="s">
         <v>64</v>
       </c>
@@ -1468,7 +1467,7 @@
       </c>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:6" ht="17.7">
+    <row r="10" spans="1:6" ht="18">
       <c r="A10" s="31" t="s">
         <v>65</v>
       </c>
@@ -1486,7 +1485,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17.7">
+    <row r="11" spans="1:6" ht="18">
       <c r="A11" s="31" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Added option to use a specified maximum acceleration distance
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Music/temp/Trajectory Sims/Git Trajectory/Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/HYPED/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51E8C60-07BE-CC4F-94B8-F02FED53D645}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B874D11-D186-7243-B23F-925B2E0C07D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1460" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1880" yWindow="1920" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="6" r:id="rId1"/>
@@ -1360,7 +1360,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="30">
-        <v>275</v>
+        <v>310</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Added functionality to cap motor torque
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/HYPED/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B874D11-D186-7243-B23F-925B2E0C07D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BE195B-676A-D949-AE92-143C5EF87545}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="1920" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="4440" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
   <si>
     <t>Parameters</t>
   </si>
@@ -313,12 +313,27 @@
   <si>
     <t>Actually 1264.92 m but rules say 1.25 km</t>
   </si>
+  <si>
+    <t>Default 0.0055</t>
+  </si>
+  <si>
+    <t>Default 111.755</t>
+  </si>
+  <si>
+    <t>Max. Torque</t>
+  </si>
+  <si>
+    <t>m_torque</t>
+  </si>
+  <si>
+    <t>N*m</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -435,6 +450,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -458,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -556,6 +577,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1309,13 +1333,14 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="37.83203125" style="1" customWidth="1"/>
-    <col min="2" max="6" width="14.1640625" style="1" customWidth="1"/>
+    <col min="2" max="5" width="14.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -1414,12 +1439,14 @@
         <v>38</v>
       </c>
       <c r="D6" s="30">
-        <v>5.4999999999999997E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="22" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="18">
       <c r="A7" s="30" t="s">
@@ -1435,7 +1462,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="30"/>
-      <c r="F7" s="23"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:6" ht="18">
       <c r="A8" s="30" t="s">
@@ -1453,7 +1480,7 @@
       <c r="E8" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="18">
       <c r="A9" s="31" t="s">
@@ -1465,13 +1492,13 @@
       <c r="C9" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="24">
-        <v>10000</v>
+      <c r="D9" s="30">
+        <v>9377</v>
       </c>
       <c r="E9" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="18">
       <c r="A10" s="31" t="s">
@@ -1483,13 +1510,14 @@
       <c r="C10" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="30">
         <f>D9*2*PI()/60</f>
-        <v>1047.1975511965977</v>
+        <v>981.95714375704972</v>
       </c>
       <c r="E10" s="31" t="s">
         <v>68</v>
       </c>
+      <c r="F10" s="22"/>
     </row>
     <row r="11" spans="1:6" ht="18">
       <c r="A11" s="31" t="s">
@@ -1501,12 +1529,33 @@
       <c r="C11" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="24">
-        <v>111.755</v>
+      <c r="D11" s="30">
+        <v>647.5</v>
       </c>
       <c r="E11" s="24" t="s">
         <v>55</v>
       </c>
+      <c r="F11" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18">
+      <c r="A12" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="30">
+        <v>25.9</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="31"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="32"/>

</xml_diff>

<commit_message>
Added motor torque calculation
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/HYPED/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BE195B-676A-D949-AE92-143C5EF87545}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1036D2C-43CF-6341-9548-D4BD55C9AB6F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="4440" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -296,9 +296,6 @@
     <t xml:space="preserve">Max. Angular Acceleration </t>
   </si>
   <si>
-    <t>Max. Rotational Frequency</t>
-  </si>
-  <si>
     <t>Max. Angular Velocity</t>
   </si>
   <si>
@@ -320,20 +317,23 @@
     <t>Default 111.755</t>
   </si>
   <si>
-    <t>Max. Torque</t>
-  </si>
-  <si>
     <t>m_torque</t>
   </si>
   <si>
     <t>N*m</t>
+  </si>
+  <si>
+    <t>Max. Motor Torque</t>
+  </si>
+  <si>
+    <t>Max. RPM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -450,6 +450,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -479,7 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -569,6 +575,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -578,7 +587,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -910,17 +919,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:9" ht="18">
       <c r="A2" s="2" t="s">
@@ -1163,14 +1172,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:6" ht="18">
       <c r="A2" s="20" t="s">
@@ -1251,13 +1260,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
       <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="19">
@@ -1301,7 +1310,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1333,7 +1342,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1345,13 +1354,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
       <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="18">
@@ -1445,7 +1454,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18">
@@ -1483,8 +1492,8 @@
       <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="18">
-      <c r="A9" s="31" t="s">
-        <v>64</v>
+      <c r="A9" s="37" t="s">
+        <v>74</v>
       </c>
       <c r="B9" s="24" t="s">
         <v>56</v>
@@ -1492,7 +1501,7 @@
       <c r="C9" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="33">
         <v>9377</v>
       </c>
       <c r="E9" s="24" t="s">
@@ -1502,20 +1511,20 @@
     </row>
     <row r="10" spans="1:6" ht="18">
       <c r="A10" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="C10" s="31" t="s">
         <v>66</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>67</v>
       </c>
       <c r="D10" s="30">
         <f>D9*2*PI()/60</f>
         <v>981.95714375704972</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F10" s="22"/>
     </row>
@@ -1529,31 +1538,31 @@
       <c r="C11" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="33">
         <v>647.5</v>
       </c>
       <c r="E11" s="24" t="s">
         <v>55</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18">
-      <c r="A12" s="31" t="s">
-        <v>72</v>
+      <c r="A12" s="37" t="s">
+        <v>73</v>
       </c>
       <c r="B12" s="31" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="30">
+        <v>71</v>
+      </c>
+      <c r="D12" s="33">
         <v>25.9</v>
       </c>
-      <c r="E12" s="36" t="s">
-        <v>74</v>
+      <c r="E12" s="37" t="s">
+        <v>72</v>
       </c>
       <c r="F12" s="31"/>
     </row>

</xml_diff>

<commit_message>
Changed force calculation to cap motor torque based on the power loss instead of net torque
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/HYPED/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1036D2C-43CF-6341-9548-D4BD55C9AB6F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAC49D2-56F3-9342-B7C1-588E635902BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="4440" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
   <si>
     <t>Parameters</t>
   </si>
@@ -311,12 +311,6 @@
     <t>Actually 1264.92 m but rules say 1.25 km</t>
   </si>
   <si>
-    <t>Default 0.0055</t>
-  </si>
-  <si>
-    <t>Default 111.755</t>
-  </si>
-  <si>
     <t>m_torque</t>
   </si>
   <si>
@@ -333,7 +327,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -450,18 +444,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -485,7 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -550,9 +532,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -575,9 +554,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -586,9 +562,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -919,17 +892,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:9" ht="18">
       <c r="A2" s="2" t="s">
@@ -1172,14 +1145,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:6" ht="18">
       <c r="A2" s="20" t="s">
@@ -1260,35 +1233,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="19">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="27"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="1:8" ht="19">
       <c r="A3" s="23" t="s">
@@ -1309,25 +1282,25 @@
       <c r="F3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="27" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1342,7 +1315,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1354,232 +1327,228 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>310</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="29" t="s">
         <v>32</v>
       </c>
       <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" ht="18">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="29">
         <v>0.06</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="29" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6" ht="18">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="29">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="29" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:6" ht="18">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="29">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="22" t="s">
-        <v>69</v>
-      </c>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="18">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="29">
         <v>5</v>
       </c>
-      <c r="E7" s="30"/>
+      <c r="E7" s="29"/>
       <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:6" ht="18">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="29">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="29" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="18">
-      <c r="A9" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="29">
         <v>9377</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="29" t="s">
         <v>57</v>
       </c>
       <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="18">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="29">
         <f>D9*2*PI()/60</f>
         <v>981.95714375704972</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="29" t="s">
         <v>67</v>
       </c>
       <c r="F10" s="22"/>
     </row>
     <row r="11" spans="1:6" ht="18">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="29">
         <v>647.5</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="1:6" ht="18">
+      <c r="A12" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="29">
+        <v>25.9</v>
+      </c>
+      <c r="E12" s="29" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="18">
-      <c r="A12" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="33">
-        <v>25.9</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="31"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="32"/>
+      <c r="A13" s="31"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="32"/>
+      <c r="A14" s="31"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="32"/>
+      <c r="A15" s="31"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="32"/>
+      <c r="A16" s="31"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="32"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>

</xml_diff>

<commit_message>
Added lookup tables for thrust force and power loss (bilinearly interpolated)
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/HYPED/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAC49D2-56F3-9342-B7C1-588E635902BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B90263D-2709-394B-9891-21E9BAFC1C5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="4440" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -261,6 +261,7 @@
         <vertAlign val="superscript"/>
         <sz val="14"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
@@ -327,7 +328,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -343,20 +344,24 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
@@ -386,6 +391,7 @@
     <font>
       <sz val="14"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -416,27 +422,32 @@
       <u/>
       <sz val="16"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
       <sz val="14"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="14"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -444,6 +455,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -467,7 +484,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -553,6 +570,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -881,7 +901,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -892,17 +912,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" ht="18">
       <c r="A2" s="2" t="s">
@@ -1145,14 +1165,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:6" ht="18">
       <c r="A2" s="20" t="s">
@@ -1233,13 +1253,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="19">
@@ -1315,7 +1335,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1327,13 +1347,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="18">
@@ -1472,8 +1492,8 @@
       <c r="C9" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="29">
-        <v>9377</v>
+      <c r="D9" s="32">
+        <v>8053</v>
       </c>
       <c r="E9" s="29" t="s">
         <v>57</v>
@@ -1492,7 +1512,7 @@
       </c>
       <c r="D10" s="29">
         <f>D9*2*PI()/60</f>
-        <v>981.95714375704972</v>
+        <v>843.30818797862014</v>
       </c>
       <c r="E10" s="29" t="s">
         <v>67</v>
@@ -1509,8 +1529,8 @@
       <c r="C11" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="29">
-        <v>647.5</v>
+      <c r="D11" s="32">
+        <v>792.5</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>55</v>
@@ -1527,8 +1547,8 @@
       <c r="C12" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="29">
-        <v>25.9</v>
+      <c r="D12" s="32">
+        <v>32.700000000000003</v>
       </c>
       <c r="E12" s="29" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Changed main calculation to a torque based approach
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/HYPED/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B90263D-2709-394B-9891-21E9BAFC1C5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196DA3A5-1884-0E47-85EC-E972682D1BD4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="4440" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19500" yWindow="8760" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="6" r:id="rId1"/>
@@ -267,12 +267,6 @@
     </r>
   </si>
   <si>
-    <t>𝛼</t>
-  </si>
-  <si>
-    <t>rad/sˆ2</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
@@ -288,15 +282,9 @@
     <t>Pod Parameters</t>
   </si>
   <si>
-    <t>m_alpha</t>
-  </si>
-  <si>
     <t>m_rpm</t>
   </si>
   <si>
-    <t xml:space="preserve">Max. Angular Acceleration </t>
-  </si>
-  <si>
     <t>Max. Angular Velocity</t>
   </si>
   <si>
@@ -322,13 +310,25 @@
   </si>
   <si>
     <t>Max. RPM</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>kg*m^2</t>
+  </si>
+  <si>
+    <t>Moment of inertia of the wheel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -455,12 +455,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -484,7 +478,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -570,9 +564,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -912,17 +903,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:9" ht="18">
       <c r="A2" s="2" t="s">
@@ -1165,14 +1156,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:6" ht="18">
       <c r="A2" s="20" t="s">
@@ -1253,13 +1244,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21">
-      <c r="A1" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="A1" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="19">
@@ -1285,7 +1276,7 @@
     </row>
     <row r="3" spans="1:8" ht="19">
       <c r="A3" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>9</v>
@@ -1303,7 +1294,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1332,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1346,17 +1337,17 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" customHeight="1">
-      <c r="A1" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+    <row r="1" spans="1:8" ht="21" customHeight="1">
+      <c r="A1" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="F1" s="15"/>
     </row>
-    <row r="2" spans="1:6" ht="18">
+    <row r="2" spans="1:8" ht="18">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
@@ -1376,7 +1367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18">
+    <row r="3" spans="1:8" ht="18">
       <c r="A3" s="29" t="s">
         <v>30</v>
       </c>
@@ -1394,7 +1385,7 @@
       </c>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:6" ht="18">
+    <row r="4" spans="1:8" ht="18">
       <c r="A4" s="29" t="s">
         <v>33</v>
       </c>
@@ -1412,7 +1403,7 @@
       </c>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6" ht="18">
+    <row r="5" spans="1:8" ht="18">
       <c r="A5" s="29" t="s">
         <v>35</v>
       </c>
@@ -1430,7 +1421,7 @@
       </c>
       <c r="F5" s="23"/>
     </row>
-    <row r="6" spans="1:6" ht="18">
+    <row r="6" spans="1:8" ht="18">
       <c r="A6" s="29" t="s">
         <v>37</v>
       </c>
@@ -1448,7 +1439,7 @@
       </c>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="18">
+    <row r="7" spans="1:8" ht="18">
       <c r="A7" s="29" t="s">
         <v>39</v>
       </c>
@@ -1464,7 +1455,7 @@
       <c r="E7" s="29"/>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="18">
+    <row r="8" spans="1:8" ht="18">
       <c r="A8" s="29" t="s">
         <v>41</v>
       </c>
@@ -1482,93 +1473,98 @@
       </c>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="18">
+    <row r="9" spans="1:8" ht="18">
       <c r="A9" s="29" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="29">
+        <v>9377</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:8" ht="18">
+      <c r="A10" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>62</v>
-      </c>
-      <c r="D9" s="32">
-        <v>8053</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" ht="18">
-      <c r="A10" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>66</v>
       </c>
       <c r="D10" s="29">
         <f>D9*2*PI()/60</f>
-        <v>843.30818797862014</v>
+        <v>981.95714375704972</v>
       </c>
       <c r="E10" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="1:8" ht="18">
+      <c r="A11" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" ht="18">
-      <c r="A11" s="29" t="s">
-        <v>63</v>
-      </c>
       <c r="B11" s="29" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="32">
-        <v>792.5</v>
+        <v>65</v>
+      </c>
+      <c r="D11" s="29">
+        <v>18.13</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" ht="18">
+        <v>66</v>
+      </c>
+      <c r="F11" s="30"/>
+    </row>
+    <row r="12" spans="1:8" ht="18">
       <c r="A12" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="29">
+        <v>0.04</v>
+      </c>
+      <c r="E12" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="32">
-        <v>32.700000000000003</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="30"/>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="31"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:8">
       <c r="A14" s="31"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:8">
       <c r="A15" s="31"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:8">
       <c r="A16" s="31"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="31"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="17"/>
+    </row>
+    <row r="17" spans="2:8">
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
@@ -1577,7 +1573,7 @@
       <c r="G17" s="15"/>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="2:8">
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -1586,7 +1582,7 @@
       <c r="G18" s="15"/>
       <c r="H18" s="17"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="2:8">
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -1595,7 +1591,7 @@
       <c r="G19" s="15"/>
       <c r="H19" s="17"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="2:8">
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -1604,7 +1600,7 @@
       <c r="G20" s="15"/>
       <c r="H20" s="17"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="2:8">
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -1613,16 +1609,16 @@
       <c r="G21" s="15"/>
       <c r="H21" s="17"/>
     </row>
-    <row r="22" spans="1:8">
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+    <row r="22" spans="2:8">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="17"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="2:8">
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -1631,7 +1627,7 @@
       <c r="G23" s="15"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="2:8">
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
@@ -1639,15 +1635,6 @@
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="17"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Improved optimal slip calculation by using a fitted polynomial
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/HYPED/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C20946-B4E8-0045-B8D8-FBF11F52C5B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FD927E-DF1E-3046-AC43-BBAD14766DAF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19500" yWindow="8760" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="4440" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="6" r:id="rId1"/>
@@ -1326,7 +1326,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1489,7 +1489,7 @@
       <c r="E9" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="22"/>
+      <c r="F9" s="29"/>
     </row>
     <row r="10" spans="1:8" ht="18">
       <c r="A10" s="29" t="s">

</xml_diff>

<commit_message>
Added inertial effects of wheel during deceleration
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/HYPED/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FD927E-DF1E-3046-AC43-BBAD14766DAF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32574CE8-21BC-4D40-A309-C32419F597E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="4440" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13200" yWindow="4580" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
   <si>
     <t>Parameters</t>
   </si>
@@ -323,16 +323,41 @@
   <si>
     <t>Moment of inertia of the wheel</t>
   </si>
+  <si>
+    <t>4 motors: 238kg, 2 motors: 163kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Number of wheel pairs</t>
+  </si>
+  <si>
+    <t>n_wheel_pairs</t>
+  </si>
+  <si>
+    <t>Number of wheels</t>
+  </si>
+  <si>
+    <t>n_wheel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -476,104 +501,105 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1326,13 +1352,15 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="37.83203125" style="1" customWidth="1"/>
-    <col min="2" max="5" width="14.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="14.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -1378,12 +1406,14 @@
         <v>31</v>
       </c>
       <c r="D3" s="29">
-        <v>310</v>
+        <v>238</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="23"/>
+      <c r="F3" s="23" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="29" t="s">
@@ -1490,6 +1520,9 @@
         <v>55</v>
       </c>
       <c r="F9" s="29"/>
+      <c r="G9" s="35" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="18">
       <c r="A10" s="29" t="s">
@@ -1521,7 +1554,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="29">
-        <v>18.13</v>
+        <v>30</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>66</v>
@@ -1545,11 +1578,32 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="31"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="31"/>
+    <row r="13" spans="1:8" ht="18">
+      <c r="A13" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="29">
+        <v>2</v>
+      </c>
+      <c r="E13" s="29"/>
+    </row>
+    <row r="14" spans="1:8" ht="18">
+      <c r="A14" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="29">
+        <f>2*D13</f>
+        <v>4</v>
+      </c>
+      <c r="E14" s="29"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="31"/>

</xml_diff>

<commit_message>
Updated braking force calculation
</commit_message>
<xml_diff>
--- a/Parameters/HalbachWheel_parameters.xlsx
+++ b/Parameters/HalbachWheel_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelanderka/Desktop/HYPED/Trajectory Sims/Git Trajectory/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32574CE8-21BC-4D40-A309-C32419F597E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A866B4A4-6817-BD4C-B42A-CC22A704743A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13200" yWindow="4580" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="4580" windowWidth="28800" windowHeight="16160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="6" r:id="rId1"/>
@@ -590,6 +590,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,7 +600,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -929,17 +929,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" ht="18">
       <c r="A2" s="2" t="s">
@@ -1182,14 +1182,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:6" ht="18">
       <c r="A2" s="20" t="s">
@@ -1270,13 +1270,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="19">
@@ -1352,7 +1352,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1366,13 +1366,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="18">
@@ -1406,7 +1406,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="29">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>32</v>
@@ -1514,13 +1514,13 @@
         <v>59</v>
       </c>
       <c r="D9" s="29">
-        <v>9377</v>
+        <v>7205</v>
       </c>
       <c r="E9" s="29" t="s">
         <v>55</v>
       </c>
       <c r="F9" s="29"/>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="32" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="D10" s="29">
         <f>D9*2*PI()/60</f>
-        <v>981.95714375704972</v>
+        <v>754.50583563714861</v>
       </c>
       <c r="E10" s="29" t="s">
         <v>63</v>
@@ -1554,7 +1554,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="29">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>66</v>

</xml_diff>